<commit_message>
'Van de Velde' i.p.v. 'Van De Velde'
</commit_message>
<xml_diff>
--- a/_data/ni/ni0708/individueel_eindstand_dworp_12_0708.xlsx
+++ b/_data/ni/ni0708/individueel_eindstand_dworp_12_0708.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" state="visible" r:id="rId2"/>
@@ -463,7 +463,7 @@
     <t xml:space="preserve">Desmedt Jean-Pierre</t>
   </si>
   <si>
-    <t xml:space="preserve">Van De Velde Filip</t>
+    <t xml:space="preserve">Van de Velde Filip</t>
   </si>
   <si>
     <t xml:space="preserve">Van Mol Yves</t>
@@ -1405,7 +1405,7 @@
   </sheetPr>
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1551,7 +1551,7 @@
   </sheetPr>
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>